<commit_message>
OPERA Reports - WIP in enhance expenses update
</commit_message>
<xml_diff>
--- a/Saudi/cancel booking.xlsx
+++ b/Saudi/cancel booking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eagle\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E7E5140-B7BB-44CD-9A8E-2970030CA68E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{952AA9B3-7941-49E3-80F8-D80EE6DCA3F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
   <si>
     <t>Booking No</t>
   </si>
@@ -64,22 +64,52 @@
     <t>Rate Code</t>
   </si>
   <si>
-    <t>DLB</t>
+    <t>PLN</t>
+  </si>
+  <si>
+    <t>MC</t>
+  </si>
+  <si>
+    <t>20.05.21</t>
+  </si>
+  <si>
+    <t>21.05.21</t>
+  </si>
+  <si>
+    <t>07.05.21</t>
+  </si>
+  <si>
+    <t>PK04972B</t>
+  </si>
+  <si>
+    <t>09.05.21</t>
+  </si>
+  <si>
+    <t>10.05.21</t>
+  </si>
+  <si>
+    <t>WHB</t>
+  </si>
+  <si>
+    <t>VA</t>
+  </si>
+  <si>
+    <t>08.05.21</t>
+  </si>
+  <si>
+    <t>11.05.21</t>
+  </si>
+  <si>
+    <t>17.05.21</t>
+  </si>
+  <si>
+    <t>RNG</t>
   </si>
   <si>
     <t>CA</t>
   </si>
   <si>
-    <t>15.05.21</t>
-  </si>
-  <si>
-    <t>17.05.21</t>
-  </si>
-  <si>
-    <t>09.05.21</t>
-  </si>
-  <si>
-    <t>HONEY1</t>
+    <t>BARBB</t>
   </si>
 </sst>
 </file>
@@ -575,16 +605,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -945,13 +972,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="18" style="1" customWidth="1"/>
@@ -960,10 +987,10 @@
     <col min="7" max="7" width="23" style="1" customWidth="1"/>
     <col min="8" max="9" width="16.140625" style="1" customWidth="1"/>
     <col min="10" max="10" width="26.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" style="1" customWidth="1"/>
     <col min="12" max="12" width="20.7109375" style="1" customWidth="1"/>
     <col min="13" max="13" width="16.5703125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="15.140625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" style="1" customWidth="1"/>
     <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1013,19 +1040,19 @@
     </row>
     <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>980469</v>
+        <v>933719</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" s="3">
         <v>1</v>
       </c>
-      <c r="E2" s="4">
-        <v>1800</v>
+      <c r="E2" s="3">
+        <v>650</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -1047,6 +1074,234 @@
       </c>
       <c r="N2" s="3" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>966969</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3">
+        <v>450</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2"/>
+      <c r="K3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>969219</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <v>450</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>969220</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3">
+        <v>450</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>964469</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3">
+        <v>450</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>968469</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3">
+        <v>450</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>968470</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3">
+        <v>450</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2"/>
+      <c r="K8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>